<commit_message>
fixing formating import parameter
</commit_message>
<xml_diff>
--- a/public/download/sampleImportParameter.xlsx
+++ b/public/download/sampleImportParameter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/logsheet_php/public/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427E8A7A-51D2-2D46-A8A9-D154D1C44293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53167669-0889-BD46-8D2C-231C8DF04048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="A1:K12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -500,10 +500,10 @@
         <v>12</v>
       </c>
       <c r="D2" s="1">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1">
         <v>56</v>
-      </c>
-      <c r="E2" s="1">
-        <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>13</v>
@@ -676,10 +676,10 @@
         <v>34</v>
       </c>
       <c r="D9" s="1">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
fixing format table parameter
</commit_message>
<xml_diff>
--- a/public/download/sampleImportParameter.xlsx
+++ b/public/download/sampleImportParameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/logsheet_php/public/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53167669-0889-BD46-8D2C-231C8DF04048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AD77E3-4152-B743-A9A4-C4333EA934DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>show on</t>
   </si>
   <si>
-    <t>TEKANAN</t>
-  </si>
-  <si>
     <t>desc 1</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>input</t>
   </si>
   <si>
-    <t>TABUNG</t>
-  </si>
-  <si>
     <t>desc 2</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t>select</t>
   </si>
   <si>
-    <t>PARAM 1</t>
-  </si>
-  <si>
     <t>desc 3</t>
   </si>
   <si>
@@ -94,15 +85,9 @@
     <t>good, bad</t>
   </si>
   <si>
-    <t>PARAM 2</t>
-  </si>
-  <si>
     <t>desc 4</t>
   </si>
   <si>
-    <t>PARAM 3</t>
-  </si>
-  <si>
     <t>desc 5</t>
   </si>
   <si>
@@ -112,24 +97,15 @@
     <t>desc 6</t>
   </si>
   <si>
-    <t>PARAM 5</t>
-  </si>
-  <si>
     <t>desc 7</t>
   </si>
   <si>
     <t>textarea</t>
   </si>
   <si>
-    <t>PARAM 6</t>
-  </si>
-  <si>
     <t>desc 8</t>
   </si>
   <si>
-    <t>PARAM 7</t>
-  </si>
-  <si>
     <t>desc 9</t>
   </si>
   <si>
@@ -145,18 +121,12 @@
     <t>Running</t>
   </si>
   <si>
-    <t>FREE TEXT</t>
-  </si>
-  <si>
     <t>DESC FREE TEXT</t>
   </si>
   <si>
     <t>checkbox</t>
   </si>
   <si>
-    <t>CHECKBOX</t>
-  </si>
-  <si>
     <t>DESC CHECKBOX</t>
   </si>
   <si>
@@ -164,13 +134,43 @@
   </si>
   <si>
     <t>Repair</t>
+  </si>
+  <si>
+    <t>Air Temperature</t>
+  </si>
+  <si>
+    <t>Barometer</t>
+  </si>
+  <si>
+    <t>Cloudness</t>
+  </si>
+  <si>
+    <t>Current and/or DR Error</t>
+  </si>
+  <si>
+    <t>Estimated Distance</t>
+  </si>
+  <si>
+    <t>Fuel Oil Consumption</t>
+  </si>
+  <si>
+    <t>Remnant at Noon</t>
+  </si>
+  <si>
+    <t>Sea Condition</t>
+  </si>
+  <si>
+    <t>Ship Draught#After</t>
+  </si>
+  <si>
+    <t>Ship Draught#Fore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,6 +197,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3C4B64"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -218,14 +229,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,12 +456,14 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="8" width="10.5703125" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" customWidth="1"/>
     <col min="10" max="26" width="10.5703125" customWidth="1"/>
   </cols>
@@ -493,11 +507,11 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>34</v>
@@ -506,79 +520,79 @@
         <v>56</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="K2" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
+      <c r="B5" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
         <v>56</v>
@@ -587,50 +601,50 @@
         <v>34</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="K5" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
+      <c r="B6" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1">
         <v>56</v>
@@ -639,41 +653,41 @@
         <v>34</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="K7" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
+      <c r="B8" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>33</v>
+      <c r="B9" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1">
         <v>32</v>
@@ -682,30 +696,30 @@
         <v>45</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="K9" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>35</v>
+      <c r="B10" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -713,22 +727,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -736,16 +750,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
formating table parameter add asset
</commit_message>
<xml_diff>
--- a/public/download/sampleImportParameter.xlsx
+++ b/public/download/sampleImportParameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/logsheet_php/public/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AD77E3-4152-B743-A9A4-C4333EA934DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FDDA7E-0F60-8E40-9477-97F486E72512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -684,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -710,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -727,7 +727,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>35</v>
@@ -750,7 +750,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>33</v>

</xml_diff>